<commit_message>
change mg_recruit output columns
</commit_message>
<xml_diff>
--- a/sag_template.xlsx
+++ b/sag_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>sag_name</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>s_wadsworthensis</t>
+  </si>
+  <si>
+    <t>fasta_file</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -432,91 +438,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="b">
+      <c r="D7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>